<commit_message>
Implemented Nutrigenomics report generation.
</commit_message>
<xml_diff>
--- a/Input/nutri_markers.xlsx
+++ b/Input/nutri_markers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Werk\Project DD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Werk\NifGo\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A56412B-1630-4F0E-A935-EDCF81ACD54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A002C46-2522-4356-8CAE-9AB502620449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="435" windowWidth="18780" windowHeight="12390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Nutri Markers 2202" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>probeset_id</t>
   </si>
@@ -64,15 +64,6 @@
     <t>ALDH2</t>
   </si>
   <si>
-    <t>AX-83376893</t>
-  </si>
-  <si>
-    <t>rs1800497</t>
-  </si>
-  <si>
-    <t>ANKK1</t>
-  </si>
-  <si>
     <t>AX-82997505</t>
   </si>
   <si>
@@ -82,12 +73,6 @@
     <t>BCO1</t>
   </si>
   <si>
-    <t>AX-11626417</t>
-  </si>
-  <si>
-    <t>rs7501331</t>
-  </si>
-  <si>
     <t>AX-11561914</t>
   </si>
   <si>
@@ -124,12 +109,6 @@
     <t>LOC105447645;FUT2</t>
   </si>
   <si>
-    <t>AX-40462051</t>
-  </si>
-  <si>
-    <t>rs602662</t>
-  </si>
-  <si>
     <t>AX-11340068</t>
   </si>
   <si>
@@ -164,15 +143,6 @@
   </si>
   <si>
     <t>NBPF3</t>
-  </si>
-  <si>
-    <t>AX-88902521</t>
-  </si>
-  <si>
-    <t>rs116855232</t>
-  </si>
-  <si>
-    <t>Nudt15</t>
   </si>
   <si>
     <t>AX-122940319</t>
@@ -1234,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,73 +1225,73 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1337,359 +1307,315 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>73</v>
-      </c>
-      <c r="C25" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="s">
         <v>81</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C29" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" t="s">
         <v>103</v>
       </c>
-      <c r="B35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>102</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
         <v>104</v>
       </c>
-      <c r="B37" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" t="s">
-        <v>114</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C30">
-    <sortCondition ref="A2:A30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C26">
+    <sortCondition ref="A2:A26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>